<commit_message>
adding keDT1 and keT1
</commit_message>
<xml_diff>
--- a/data/Bx_Atezolizumab.xlsx
+++ b/data/Bx_Atezolizumab.xlsx
@@ -15,26 +15,26 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ABCdrug">Sheet1!$F$41</definedName>
-    <definedName name="ABCsol">Sheet1!$F$42</definedName>
+    <definedName name="ABCdrug">Sheet1!$F$43</definedName>
+    <definedName name="ABCsol">Sheet1!$F$44</definedName>
     <definedName name="CL">Sheet1!$F$4</definedName>
-    <definedName name="eps">Sheet1!$F$46</definedName>
+    <definedName name="eps">Sheet1!$F$48</definedName>
     <definedName name="k12D">Sheet1!$F$11</definedName>
-    <definedName name="k13D">Sheet1!$F$47</definedName>
-    <definedName name="k13DS">Sheet1!$F$49</definedName>
-    <definedName name="k13S">Sheet1!$F$48</definedName>
+    <definedName name="k13D">Sheet1!$F$49</definedName>
+    <definedName name="k13DS">Sheet1!$F$51</definedName>
+    <definedName name="k13S">Sheet1!$F$50</definedName>
     <definedName name="k21D">Sheet1!$F$12</definedName>
     <definedName name="Kd">Sheet1!$F$16</definedName>
     <definedName name="keD">Sheet1!$F$5</definedName>
-    <definedName name="keT3_">Sheet1!$F$39</definedName>
+    <definedName name="keT3_">Sheet1!$F$41</definedName>
     <definedName name="koff">Sheet1!$F$16</definedName>
     <definedName name="kshed">Sheet1!$F$31</definedName>
     <definedName name="Npercell">Sheet1!$F$25</definedName>
-    <definedName name="P">Sheet1!$F$43</definedName>
+    <definedName name="P">Sheet1!$F$45</definedName>
     <definedName name="Q">Sheet1!$F$6</definedName>
-    <definedName name="Rcap">Sheet1!$F$44</definedName>
+    <definedName name="Rcap">Sheet1!$F$46</definedName>
     <definedName name="Rho">Sheet1!$F$26</definedName>
-    <definedName name="Rkrogh">Sheet1!$F$45</definedName>
+    <definedName name="Rkrogh">Sheet1!$F$47</definedName>
     <definedName name="T30_">Sheet1!$F$28</definedName>
     <definedName name="Tfrac">Sheet1!$F$27</definedName>
     <definedName name="Vc">Sheet1!$F$7</definedName>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="136">
   <si>
     <t>Parameter</t>
   </si>
@@ -460,6 +460,12 @@
   </si>
   <si>
     <t>assumed same as target</t>
+  </si>
+  <si>
+    <t>keT1</t>
+  </si>
+  <si>
+    <t>keDT1</t>
   </si>
 </sst>
 </file>
@@ -977,10 +983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2034,50 +2040,32 @@
       <c r="I38" s="12"/>
     </row>
     <row r="39" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="15">
-        <v>30</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="F39" s="6">
-        <f>LN(2)/1</f>
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F39" s="7">
+        <f>keT3_</f>
         <v>0.69314718055994529</v>
       </c>
-      <c r="G39" s="5" t="s">
+      <c r="G39" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H39" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="I39" s="16" t="s">
-        <v>132</v>
-      </c>
+      <c r="H39" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I39" s="12"/>
     </row>
     <row r="40" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="11">
-        <v>31</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>88</v>
-      </c>
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
       <c r="E40" s="4" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="F40" s="7">
         <f>F39</f>
@@ -2087,313 +2075,371 @@
         <v>4</v>
       </c>
       <c r="H40" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I40" s="12"/>
+    </row>
+    <row r="41" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="15">
+        <v>30</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F41" s="6">
+        <f>LN(2)/1</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H41" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="I40" s="12" t="s">
+      <c r="I41" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="11">
+        <v>31</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F42" s="7">
+        <f>F41</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I42" s="12" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="11">
-        <v>32</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="11">
-        <v>33</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="11">
+        <v>32</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="11">
+        <v>33</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="11">
         <v>33.1</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F43" s="22">
+      <c r="F45" s="22">
         <f>0.000000003*1000000*60*60*24</f>
         <v>259.2</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="I43" s="14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="11">
-        <v>33.200000000000003</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F44" s="6">
-        <v>8</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I44" s="14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="11">
-        <v>33.299999999999997</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F45" s="6">
-        <v>75</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="I45" s="14" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="11"/>
+      <c r="A46" s="11">
+        <v>33.200000000000003</v>
+      </c>
       <c r="E46" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F46" s="6">
-        <v>0.24</v>
+        <v>8</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="I46" s="14" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="11">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F47" s="6">
+        <v>75</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I47" s="14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="11"/>
+      <c r="E48" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F48" s="6">
+        <v>0.24</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I48" s="14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="11">
         <v>34</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B49" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C49" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D47" s="11" t="s">
+      <c r="D49" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E49" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="7">
+      <c r="F49" s="7">
         <f>2*P*Rcap/Rkrogh^2</f>
         <v>0.73727999999999994</v>
       </c>
-      <c r="G47" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I47" s="12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="11">
-        <v>35</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H48" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I48" s="12"/>
-    </row>
-    <row r="49" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="11">
-        <v>36</v>
-      </c>
-      <c r="B49" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="G49" s="4" t="s">
         <v>4</v>
       </c>
       <c r="H49" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="I49" s="12"/>
+      <c r="I49" s="12" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="50" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="11">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B50" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C50" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I50" s="12"/>
+    </row>
+    <row r="51" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="11">
+        <v>36</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I51" s="12"/>
+    </row>
+    <row r="52" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="11">
+        <v>37</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D50" s="11" t="s">
+      <c r="D52" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="E52" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F50" s="7">
+      <c r="F52" s="7">
         <f>k13D</f>
         <v>0.73727999999999994</v>
       </c>
-      <c r="G50" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I50" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="11">
-        <v>38</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H51" s="11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="11">
-        <v>39</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D52" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="G52" s="4" t="s">
         <v>4</v>
       </c>
       <c r="H52" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="I52" s="12"/>
+      <c r="I52" s="12" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="53" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="H53" s="11"/>
+      <c r="A53" s="11">
+        <v>38</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H53" s="11" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="54" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="H54" s="4"/>
+      <c r="A54" s="11">
+        <v>39</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="I54" s="12"/>
     </row>
-    <row r="59" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="F59" s="12"/>
-      <c r="H59" s="11"/>
+    <row r="55" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H55" s="11"/>
+    </row>
+    <row r="56" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H56" s="4"/>
+      <c r="I56" s="12"/>
+    </row>
+    <row r="61" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F61" s="12"/>
+      <c r="H61" s="11"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F276">
+  <conditionalFormatting sqref="F278">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="derived">
-      <formula>NOT(ISERROR(SEARCH("derived",F276)))</formula>
+      <formula>NOT(ISERROR(SEARCH("derived",F278)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>